<commit_message>
New plots and folder
</commit_message>
<xml_diff>
--- a/OUTtoShare/Passerine_diversity_by_group.xlsx
+++ b/OUTtoShare/Passerine_diversity_by_group.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>ID_PSU</t>
   </si>
@@ -64,15 +64,6 @@
     <t>Feed_Insectivorous_sum</t>
   </si>
   <si>
-    <t>Feed_Omnivorous_sum</t>
-  </si>
-  <si>
-    <t>Omnivorous_h3_sum</t>
-  </si>
-  <si>
-    <t>Omnivorous_prev_sum</t>
-  </si>
-  <si>
     <t>Nest_Tree_sum</t>
   </si>
   <si>
@@ -176,6 +167,18 @@
   </si>
   <si>
     <t xml:space="preserve">85 </t>
+  </si>
+  <si>
+    <t>Feed_Omn_sum</t>
+  </si>
+  <si>
+    <t>Feed_Omn_h3_sum</t>
+  </si>
+  <si>
+    <t>Feed_Omn_prev_sum</t>
+  </si>
+  <si>
+    <t>Feed_Omn_Omn_h3_sum</t>
   </si>
 </sst>
 </file>
@@ -525,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD25"/>
+  <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,20 +555,21 @@
     <col min="17" max="17" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="20" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="22" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="21" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="21" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -615,51 +619,54 @@
         <v>15</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>27</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>30</v>
       </c>
       <c r="B2">
         <v>16</v>
@@ -716,42 +723,45 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="U2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="V2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="W2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="X2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="Y2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="Z2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AA2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AB2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AC2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AD2">
         <v>4</v>
       </c>
+      <c r="AE2">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <v>20</v>
@@ -808,31 +818,31 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="U3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="V3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="W3">
+        <v>3</v>
+      </c>
+      <c r="X3">
         <v>9</v>
       </c>
-      <c r="X3">
-        <v>5</v>
-      </c>
       <c r="Y3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="Z3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA3">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="AB3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AC3">
         <v>4</v>
@@ -840,10 +850,13 @@
       <c r="AD3">
         <v>4</v>
       </c>
+      <c r="AE3">
+        <v>4</v>
+      </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <v>17</v>
@@ -900,42 +913,45 @@
         <v>2</v>
       </c>
       <c r="T4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U4">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="V4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W4">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="X4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="Y4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Z4">
         <v>1</v>
       </c>
       <c r="AA4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AB4">
         <v>5</v>
       </c>
       <c r="AC4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AD4">
+        <v>4</v>
+      </c>
+      <c r="AE4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B5">
         <v>20</v>
@@ -992,42 +1008,45 @@
         <v>1</v>
       </c>
       <c r="T5">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="U5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="V5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="W5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="X5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Z5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA5">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AB5">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AC5">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AD5">
+        <v>4</v>
+      </c>
+      <c r="AE5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B6">
         <v>12</v>
@@ -1084,42 +1103,45 @@
         <v>0</v>
       </c>
       <c r="T6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U6">
         <v>4</v>
       </c>
       <c r="V6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="X6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Y6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Z6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AB6">
         <v>4</v>
       </c>
       <c r="AC6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AD6">
+        <v>3</v>
+      </c>
+      <c r="AE6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B7">
         <v>20</v>
@@ -1179,39 +1201,42 @@
         <v>8</v>
       </c>
       <c r="U7">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="V7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="W7">
+        <v>3</v>
+      </c>
+      <c r="X7">
         <v>11</v>
       </c>
-      <c r="X7">
-        <v>5</v>
-      </c>
       <c r="Y7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Z7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AA7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AB7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AD7">
+        <v>4</v>
+      </c>
+      <c r="AE7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <v>14</v>
@@ -1271,39 +1296,42 @@
         <v>2</v>
       </c>
       <c r="U8">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="V8">
         <v>5</v>
       </c>
       <c r="W8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="X8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Z8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA8">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AB8">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AC8">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AD8">
+        <v>6</v>
+      </c>
+      <c r="AE8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B9">
         <v>21</v>
@@ -1369,33 +1397,36 @@
         <v>6</v>
       </c>
       <c r="W9">
+        <v>6</v>
+      </c>
+      <c r="X9">
         <v>9</v>
       </c>
-      <c r="X9">
-        <v>4</v>
-      </c>
       <c r="Y9">
         <v>4</v>
       </c>
       <c r="Z9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AA9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AB9">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AC9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AD9">
+        <v>7</v>
+      </c>
+      <c r="AE9">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B10">
         <v>16</v>
@@ -1452,42 +1483,45 @@
         <v>0</v>
       </c>
       <c r="T10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W10">
+        <v>4</v>
+      </c>
+      <c r="X10">
         <v>9</v>
       </c>
-      <c r="X10">
-        <v>5</v>
-      </c>
       <c r="Y10">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="Z10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA10">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="AB10">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AC10">
         <v>4</v>
       </c>
       <c r="AD10">
+        <v>4</v>
+      </c>
+      <c r="AE10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B11">
         <v>14</v>
@@ -1544,42 +1578,45 @@
         <v>1</v>
       </c>
       <c r="T11">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U11">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="V11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="W11">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="X11">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Y11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Z11">
         <v>1</v>
       </c>
       <c r="AA11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AC11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AD11">
+        <v>3</v>
+      </c>
+      <c r="AE11">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B12">
         <v>17</v>
@@ -1636,42 +1673,45 @@
         <v>1</v>
       </c>
       <c r="T12">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="U12">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="V12">
         <v>3</v>
       </c>
       <c r="W12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="X12">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="Y12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Z12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AA12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AB12">
         <v>4</v>
       </c>
       <c r="AC12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AD12">
+        <v>5</v>
+      </c>
+      <c r="AE12">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B13">
         <v>14</v>
@@ -1731,39 +1771,42 @@
         <v>6</v>
       </c>
       <c r="U13">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="V13">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="W13">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="X13">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Y13">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="Z13">
         <v>2</v>
       </c>
       <c r="AA13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AB13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AC13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AD13">
+        <v>3</v>
+      </c>
+      <c r="AE13">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B14">
         <v>18</v>
@@ -1820,42 +1863,45 @@
         <v>2</v>
       </c>
       <c r="T14">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="U14">
         <v>5</v>
       </c>
       <c r="V14">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="W14">
+        <v>2</v>
+      </c>
+      <c r="X14">
         <v>10</v>
       </c>
-      <c r="X14">
-        <v>6</v>
-      </c>
       <c r="Y14">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="Z14">
         <v>3</v>
       </c>
       <c r="AA14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AB14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AC14">
         <v>4</v>
       </c>
       <c r="AD14">
+        <v>4</v>
+      </c>
+      <c r="AE14">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B15">
         <v>20</v>
@@ -1915,39 +1961,42 @@
         <v>6</v>
       </c>
       <c r="U15">
+        <v>6</v>
+      </c>
+      <c r="V15">
         <v>9</v>
       </c>
-      <c r="V15">
-        <v>5</v>
-      </c>
       <c r="W15">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="X15">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Y15">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Z15">
         <v>1</v>
       </c>
       <c r="AA15">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="AB15">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AC15">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="AD15">
+        <v>7</v>
+      </c>
+      <c r="AE15">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B16">
         <v>9</v>
@@ -2004,10 +2053,10 @@
         <v>0</v>
       </c>
       <c r="T16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="U16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V16">
         <v>3</v>
@@ -2019,27 +2068,30 @@
         <v>3</v>
       </c>
       <c r="Y16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Z16">
         <v>0</v>
       </c>
       <c r="AA16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AC16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AD16">
+        <v>2</v>
+      </c>
+      <c r="AE16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B17">
         <v>11</v>
@@ -2096,42 +2148,45 @@
         <v>2</v>
       </c>
       <c r="T17">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U17">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="V17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="X17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Y17">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Z17">
         <v>0</v>
       </c>
       <c r="AA17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB17">
         <v>2</v>
       </c>
       <c r="AC17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AD17">
+        <v>3</v>
+      </c>
+      <c r="AE17">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B18">
         <v>25</v>
@@ -2188,42 +2243,45 @@
         <v>3</v>
       </c>
       <c r="T18">
+        <v>9</v>
+      </c>
+      <c r="U18">
         <v>11</v>
       </c>
-      <c r="U18">
-        <v>7</v>
-      </c>
       <c r="V18">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="W18">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="X18">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Y18">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="Z18">
         <v>2</v>
       </c>
       <c r="AA18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AB18">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AC18">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AD18">
+        <v>6</v>
+      </c>
+      <c r="AE18">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B19">
         <v>20</v>
@@ -2280,28 +2338,28 @@
         <v>3</v>
       </c>
       <c r="T19">
+        <v>8</v>
+      </c>
+      <c r="U19">
         <v>10</v>
       </c>
-      <c r="U19">
-        <v>6</v>
-      </c>
       <c r="V19">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="W19">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="X19">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="Y19">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="Z19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA19">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AB19">
         <v>5</v>
@@ -2312,10 +2370,13 @@
       <c r="AD19">
         <v>5</v>
       </c>
+      <c r="AE19">
+        <v>5</v>
+      </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B20">
         <v>23</v>
@@ -2378,36 +2439,39 @@
         <v>7</v>
       </c>
       <c r="V20">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="W20">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="X20">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="Y20">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Z20">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AA20">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="AB20">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AC20">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="AD20">
+        <v>5</v>
+      </c>
+      <c r="AE20">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B21">
         <v>13</v>
@@ -2464,42 +2528,45 @@
         <v>0</v>
       </c>
       <c r="T21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U21">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="V21">
         <v>5</v>
       </c>
       <c r="W21">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="X21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AA21">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AB21">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AC21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AD21">
+        <v>4</v>
+      </c>
+      <c r="AE21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B22">
         <v>8</v>
@@ -2556,42 +2623,45 @@
         <v>0</v>
       </c>
       <c r="T22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="V22">
         <v>4</v>
       </c>
       <c r="W22">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="X22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AC22">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD22">
+        <v>2</v>
+      </c>
+      <c r="AE22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B23">
         <v>19</v>
@@ -2648,42 +2718,45 @@
         <v>0</v>
       </c>
       <c r="T23">
+        <v>1</v>
+      </c>
+      <c r="U23">
         <v>9</v>
       </c>
-      <c r="U23">
+      <c r="V23">
         <v>11</v>
       </c>
-      <c r="V23">
-        <v>5</v>
-      </c>
       <c r="W23">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="X23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z23">
         <v>0</v>
       </c>
       <c r="AA23">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AB23">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="AC23">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AD23">
+        <v>4</v>
+      </c>
+      <c r="AE23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B24">
         <v>13</v>
@@ -2740,42 +2813,45 @@
         <v>1</v>
       </c>
       <c r="T24">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="U24">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="V24">
         <v>4</v>
       </c>
       <c r="W24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="X24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z24">
         <v>0</v>
       </c>
       <c r="AA24">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AB24">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AC24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AD24">
         <v>3</v>
       </c>
+      <c r="AE24">
+        <v>3</v>
+      </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -2835,33 +2911,36 @@
         <v>6</v>
       </c>
       <c r="U25">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="V25">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="W25">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="X25">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Y25">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="Z25">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AA25">
+        <v>2</v>
+      </c>
+      <c r="AB25">
         <v>9</v>
       </c>
-      <c r="AB25">
-        <v>7</v>
-      </c>
       <c r="AC25">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AD25">
+        <v>6</v>
+      </c>
+      <c r="AE25">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Modified column names (whitespaces removed)"
This reverts commit f56e13395efc236761e6bfe96f22a0ed2bec47ff.
</commit_message>
<xml_diff>
--- a/OUTtoShare/Passerine_diversity_by_group.xlsx
+++ b/OUTtoShare/Passerine_diversity_by_group.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocs\R-dev\Thesis\OUTtoShare\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288CEE3C-A833-4A4F-BE21-ACAEA4F80636}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -88,6 +82,12 @@
     <t>Nest_Ground_sum</t>
   </si>
   <si>
+    <t>Nest_Artificial Urban_sum</t>
+  </si>
+  <si>
+    <t>Nest_Tree Cavity_sum</t>
+  </si>
+  <si>
     <t>Nest_Cavity_sum</t>
   </si>
   <si>
@@ -176,18 +176,12 @@
   </si>
   <si>
     <t xml:space="preserve">85 </t>
-  </si>
-  <si>
-    <t>Nest_Artificial_Urban_sum</t>
-  </si>
-  <si>
-    <t>Nest_Tree_Cavity_sum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -240,9 +234,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -290,7 +281,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -323,26 +314,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -375,23 +349,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -567,11 +524,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,33 +633,33 @@
         <v>21</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>16</v>
@@ -794,7 +751,7 @@
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>20</v>
@@ -886,7 +843,7 @@
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B4">
         <v>17</v>
@@ -978,7 +935,7 @@
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B5">
         <v>20</v>
@@ -1070,7 +1027,7 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B6">
         <v>12</v>
@@ -1162,7 +1119,7 @@
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B7">
         <v>20</v>
@@ -1254,7 +1211,7 @@
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B8">
         <v>14</v>
@@ -1346,7 +1303,7 @@
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B9">
         <v>21</v>
@@ -1438,7 +1395,7 @@
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B10">
         <v>16</v>
@@ -1530,7 +1487,7 @@
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B11">
         <v>14</v>
@@ -1622,7 +1579,7 @@
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B12">
         <v>17</v>
@@ -1714,7 +1671,7 @@
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B13">
         <v>14</v>
@@ -1806,7 +1763,7 @@
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B14">
         <v>18</v>
@@ -1898,7 +1855,7 @@
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B15">
         <v>20</v>
@@ -1990,7 +1947,7 @@
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B16">
         <v>9</v>
@@ -2082,7 +2039,7 @@
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B17">
         <v>11</v>
@@ -2174,7 +2131,7 @@
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B18">
         <v>25</v>
@@ -2266,7 +2223,7 @@
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B19">
         <v>20</v>
@@ -2358,7 +2315,7 @@
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B20">
         <v>23</v>
@@ -2450,7 +2407,7 @@
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B21">
         <v>13</v>
@@ -2542,7 +2499,7 @@
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B22">
         <v>8</v>
@@ -2634,7 +2591,7 @@
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B23">
         <v>19</v>
@@ -2726,7 +2683,7 @@
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B24">
         <v>13</v>
@@ -2818,7 +2775,7 @@
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B25">
         <v>24</v>

</xml_diff>

<commit_message>
Modified column names (whitespaces removed)
</commit_message>
<xml_diff>
--- a/OUTtoShare/Passerine_diversity_by_group.xlsx
+++ b/OUTtoShare/Passerine_diversity_by_group.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocs\R-dev\Thesis\OUTtoShare\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288CEE3C-A833-4A4F-BE21-ACAEA4F80636}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -82,12 +88,6 @@
     <t>Nest_Ground_sum</t>
   </si>
   <si>
-    <t>Nest_Artificial Urban_sum</t>
-  </si>
-  <si>
-    <t>Nest_Tree Cavity_sum</t>
-  </si>
-  <si>
     <t>Nest_Cavity_sum</t>
   </si>
   <si>
@@ -176,12 +176,18 @@
   </si>
   <si>
     <t xml:space="preserve">85 </t>
+  </si>
+  <si>
+    <t>Nest_Artificial_Urban_sum</t>
+  </si>
+  <si>
+    <t>Nest_Tree_Cavity_sum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -234,6 +240,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -281,7 +290,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -314,9 +323,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -349,6 +375,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -524,11 +567,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,33 +676,33 @@
         <v>21</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>16</v>
@@ -751,7 +794,7 @@
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>20</v>
@@ -843,7 +886,7 @@
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <v>17</v>
@@ -935,7 +978,7 @@
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5">
         <v>20</v>
@@ -1027,7 +1070,7 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6">
         <v>12</v>
@@ -1119,7 +1162,7 @@
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B7">
         <v>20</v>
@@ -1211,7 +1254,7 @@
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B8">
         <v>14</v>
@@ -1303,7 +1346,7 @@
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B9">
         <v>21</v>
@@ -1395,7 +1438,7 @@
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B10">
         <v>16</v>
@@ -1487,7 +1530,7 @@
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B11">
         <v>14</v>
@@ -1579,7 +1622,7 @@
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B12">
         <v>17</v>
@@ -1671,7 +1714,7 @@
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B13">
         <v>14</v>
@@ -1763,7 +1806,7 @@
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14">
         <v>18</v>
@@ -1855,7 +1898,7 @@
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B15">
         <v>20</v>
@@ -1947,7 +1990,7 @@
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B16">
         <v>9</v>
@@ -2039,7 +2082,7 @@
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B17">
         <v>11</v>
@@ -2131,7 +2174,7 @@
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B18">
         <v>25</v>
@@ -2223,7 +2266,7 @@
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B19">
         <v>20</v>
@@ -2315,7 +2358,7 @@
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B20">
         <v>23</v>
@@ -2407,7 +2450,7 @@
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B21">
         <v>13</v>
@@ -2499,7 +2542,7 @@
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B22">
         <v>8</v>
@@ -2591,7 +2634,7 @@
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B23">
         <v>19</v>
@@ -2683,7 +2726,7 @@
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B24">
         <v>13</v>
@@ -2775,7 +2818,7 @@
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B25">
         <v>24</v>

</xml_diff>